<commit_message>
PreCompiled methods are quick...
</commit_message>
<xml_diff>
--- a/VirtualObjects.Tests/Performance.xlsx
+++ b/VirtualObjects.Tests/Performance.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
-    <sheet name="Factory" sheetId="4" r:id="rId1"/>
+    <sheet name="EntitiesMapping" sheetId="6" r:id="rId1"/>
+    <sheet name="EntitiesCreation" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>NumberOfEntities</t>
   </si>
@@ -39,6 +40,24 @@
   </si>
   <si>
     <t>Activator</t>
+  </si>
+  <si>
+    <t>Pooling</t>
+  </si>
+  <si>
+    <t>SetFieldFinalValue</t>
+  </si>
+  <si>
+    <t>SetValue</t>
+  </si>
+  <si>
+    <t>HardCoded</t>
+  </si>
+  <si>
+    <t>Parallel</t>
+  </si>
+  <si>
+    <t>Compiled</t>
   </si>
 </sst>
 </file>
@@ -128,11 +147,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Factory!$C$1</c:f>
+              <c:f>EntitiesMapping!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>New</c:v>
+                  <c:v>SetValue</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -157,7 +176,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Factory!$A$2:$A$50</c:f>
+              <c:f>EntitiesMapping!$A$2:$A$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="49"/>
@@ -166,7 +185,59 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Factory!$C$3:$C$50</c:f>
+              <c:f>EntitiesMapping!$C$3:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="48"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EntitiesMapping!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SetFieldFinalValue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>EntitiesMapping!$A$2:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="49"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EntitiesMapping!$B$3:$B$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="48"/>
@@ -177,14 +248,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Factory!$D$1</c:f>
+              <c:f>EntitiesMapping!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fasterflect</c:v>
+                  <c:v>HardCoded</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -209,7 +280,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Factory!$A$2:$A$50</c:f>
+              <c:f>EntitiesMapping!$A$2:$A$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="49"/>
@@ -218,9 +289,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Factory!$D$3:$D$50</c:f>
+              <c:f>EntitiesMapping!$D$3:$D$50</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
               </c:numCache>
             </c:numRef>
@@ -229,14 +300,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Factory!$E$1</c:f>
+              <c:f>EntitiesMapping!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Activator</c:v>
+                  <c:v>Parallel</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -261,7 +332,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Factory!$A$2:$A$50</c:f>
+              <c:f>EntitiesMapping!$A$2:$A$50</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="49"/>
@@ -270,9 +341,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Factory!$E$3:$E$50</c:f>
+              <c:f>EntitiesMapping!$E$3:$E$50</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
               </c:numCache>
             </c:numRef>
@@ -280,15 +351,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="3"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Factory!$B$1</c:f>
+              <c:f>EntitiesMapping!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>EntityProvider</c:v>
+                  <c:v>Compiled</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -296,7 +367,7 @@
           <c:spPr>
             <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -311,20 +382,11 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Factory!$A$2:$A$50</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="49"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Factory!$B$3:$B$50</c:f>
+              <c:f>EntitiesMapping!$F$3:$F$50</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
               </c:numCache>
             </c:numRef>
@@ -340,11 +402,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="228822520"/>
-        <c:axId val="228822912"/>
+        <c:axId val="228898400"/>
+        <c:axId val="228892520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="228822520"/>
+        <c:axId val="228898400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -386,7 +448,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228822912"/>
+        <c:crossAx val="228892520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -394,7 +456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228822912"/>
+        <c:axId val="228892520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -444,7 +506,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228822520"/>
+        <c:crossAx val="228898400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -459,6 +521,480 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EntitiesCreation!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>New</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>EntitiesCreation!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="40"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EntitiesCreation!$C$2:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="40"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EntitiesCreation!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fasterflect</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>EntitiesCreation!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="40"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EntitiesCreation!$D$2:$D$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="40"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EntitiesCreation!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Activator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>EntitiesCreation!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="40"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EntitiesCreation!$E$2:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="40"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EntitiesCreation!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EntityProvider</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>EntitiesCreation!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="40"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EntitiesCreation!$B$2:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="40"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EntitiesCreation!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pooling</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>EntitiesCreation!$F$2:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="301523856"/>
+        <c:axId val="301521504"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="301523856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="301521504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="301521504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="301523856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -575,6 +1111,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -1071,20 +1647,553 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>128586</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1371,10 +2480,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,6 +2533,7 @@
     <col min="1" max="2" width="16.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
     <col min="4" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1400,6 +2552,9 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>

</xml_diff>